<commit_message>
updated HLCM to cmdstanr
</commit_message>
<xml_diff>
--- a/1_HLCM/Figs_Tables/Key.xlsx
+++ b/1_HLCM/Figs_Tables/Key.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmh31\OneDrive - Temple University\Temple\IGT Papers &amp; Data\IGT_PP_Shared\1_HLCM\Figs_Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA59EABA-2A98-4297-AC79-7EFA05561908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69B85522-33BA-425B-9059-D439CA1CE828}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-5280" windowWidth="23256" windowHeight="12456" xr2:uid="{C68C78FF-C6FC-4D02-B882-8B55A225AB78}"/>
+    <workbookView xWindow="-108" yWindow="-14508" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{C68C78FF-C6FC-4D02-B882-8B55A225AB78}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="RL Simulation" sheetId="1" r:id="rId1"/>
+    <sheet name="TADS Dataframe" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="100">
   <si>
     <t>condition</t>
   </si>
@@ -186,13 +187,163 @@
   </si>
   <si>
     <t>DIAGNOSTICS</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>participant</t>
+  </si>
+  <si>
+    <t>platform</t>
+  </si>
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>card</t>
+  </si>
+  <si>
+    <t>block</t>
+  </si>
+  <si>
+    <t>trial</t>
+  </si>
+  <si>
+    <t>card_good</t>
+  </si>
+  <si>
+    <t>card_RT</t>
+  </si>
+  <si>
+    <t>card_play</t>
+  </si>
+  <si>
+    <t>outcome</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>AB_card</t>
+  </si>
+  <si>
+    <t>checked_version</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>dad</t>
+  </si>
+  <si>
+    <t>in-person</t>
+  </si>
+  <si>
+    <t>AB</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>AB_D</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>AB_A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>AB_B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>AB_C</t>
+  </si>
+  <si>
+    <t>Data Type:</t>
+  </si>
+  <si>
+    <t>Example Data:</t>
+  </si>
+  <si>
+    <t>Variable:</t>
+  </si>
+  <si>
+    <t>Explanation of Data:</t>
+  </si>
+  <si>
+    <t>participant ID</t>
+  </si>
+  <si>
+    <t>session (T1-T5)</t>
+  </si>
+  <si>
+    <t>mom/dad/child</t>
+  </si>
+  <si>
+    <t>whether data were collected in person (Eprime) or online (Pavlovia)</t>
+  </si>
+  <si>
+    <t>AB/BD</t>
+  </si>
+  <si>
+    <t>block of trials (1-3</t>
+  </si>
+  <si>
+    <t>trial in whole task (1-120)</t>
+  </si>
+  <si>
+    <t>0 = bad card; 1 = good card</t>
+  </si>
+  <si>
+    <t>reaction time (4000 = automatic pass)</t>
+  </si>
+  <si>
+    <t>0 = passed; 1 = played</t>
+  </si>
+  <si>
+    <t>outcome from choice</t>
+  </si>
+  <si>
+    <t>date of administration</t>
+  </si>
+  <si>
+    <t>normalized card (i.e., BD cards have been recoded as their corresponding AB cards)</t>
+  </si>
+  <si>
+    <t>version checked by looking at sequence of outcomes</t>
+  </si>
+  <si>
+    <t>character</t>
+  </si>
+  <si>
+    <t>numeric</t>
+  </si>
+  <si>
+    <t>posterior_SD</t>
+  </si>
+  <si>
+    <t>card name presented on task (cards will differ across versions)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -202,6 +353,15 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -288,14 +448,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -643,50 +803,48 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DD738D5-3997-4845-9801-7133B0A02820}">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="8.7265625" style="2"/>
-    <col min="2" max="4" width="8.7265625" style="3"/>
-    <col min="5" max="5" width="8.7265625" style="4"/>
-    <col min="6" max="6" width="8.7265625" style="2"/>
-    <col min="7" max="9" width="8.7265625" style="3"/>
-    <col min="10" max="10" width="8.7265625" style="4"/>
+    <col min="5" max="5" width="8.7265625" style="3"/>
+    <col min="6" max="6" width="14.08984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.7265625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="8" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:12" s="7" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="5" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="6" t="s">
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="5" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" t="s">
         <v>23</v>
       </c>
       <c r="K2" s="1" t="s">
@@ -697,16 +855,16 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" t="s">
         <v>24</v>
       </c>
       <c r="K3" s="1" t="s">
@@ -717,166 +875,166 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" t="s">
         <v>34</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="L4" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" t="s">
         <v>35</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L5" s="9" t="s">
+      <c r="L5" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" t="s">
         <v>36</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="L6" s="9" t="s">
+      <c r="L6" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" t="s">
         <v>37</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L7" s="9" t="s">
+      <c r="L7" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="G8" t="s">
         <v>40</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L8" s="9" t="s">
+      <c r="L8" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" t="s">
         <v>30</v>
       </c>
-      <c r="F9" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" s="9" t="s">
+      <c r="F9" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="G9" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="G10" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" t="s">
         <v>32</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="G11" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" t="s">
         <v>31</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F12" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="G12" s="9" t="s">
+      <c r="G12" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="G13" t="s">
         <v>43</v>
       </c>
     </row>
@@ -886,4 +1044,506 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EBB961D-66F4-4197-909B-2BCEDE4707AF}">
+  <dimension ref="A1:P10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="17.08984375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="N1" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="O1" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="P1" s="10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H2" t="s">
+        <v>87</v>
+      </c>
+      <c r="I2" t="s">
+        <v>88</v>
+      </c>
+      <c r="J2" t="s">
+        <v>89</v>
+      </c>
+      <c r="K2" t="s">
+        <v>90</v>
+      </c>
+      <c r="L2" t="s">
+        <v>91</v>
+      </c>
+      <c r="M2" t="s">
+        <v>92</v>
+      </c>
+      <c r="N2" t="s">
+        <v>93</v>
+      </c>
+      <c r="O2" t="s">
+        <v>94</v>
+      </c>
+      <c r="P2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F3" t="s">
+        <v>96</v>
+      </c>
+      <c r="G3" t="s">
+        <v>96</v>
+      </c>
+      <c r="H3" t="s">
+        <v>97</v>
+      </c>
+      <c r="I3" t="s">
+        <v>97</v>
+      </c>
+      <c r="J3" t="s">
+        <v>97</v>
+      </c>
+      <c r="K3" t="s">
+        <v>97</v>
+      </c>
+      <c r="L3" t="s">
+        <v>97</v>
+      </c>
+      <c r="M3" t="s">
+        <v>97</v>
+      </c>
+      <c r="N3" t="s">
+        <v>96</v>
+      </c>
+      <c r="O3" t="s">
+        <v>96</v>
+      </c>
+      <c r="P3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H4" t="s">
+        <v>56</v>
+      </c>
+      <c r="I4" t="s">
+        <v>57</v>
+      </c>
+      <c r="J4" t="s">
+        <v>58</v>
+      </c>
+      <c r="K4" t="s">
+        <v>59</v>
+      </c>
+      <c r="L4" t="s">
+        <v>60</v>
+      </c>
+      <c r="M4" t="s">
+        <v>61</v>
+      </c>
+      <c r="N4" t="s">
+        <v>62</v>
+      </c>
+      <c r="O4" t="s">
+        <v>63</v>
+      </c>
+      <c r="P4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B5">
+        <v>5002</v>
+      </c>
+      <c r="C5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F5" t="s">
+        <v>68</v>
+      </c>
+      <c r="G5" t="s">
+        <v>69</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>4000</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5" t="s">
+        <v>70</v>
+      </c>
+      <c r="N5" s="9">
+        <v>42645</v>
+      </c>
+      <c r="O5" t="s">
+        <v>71</v>
+      </c>
+      <c r="P5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B6">
+        <v>5002</v>
+      </c>
+      <c r="C6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F6" t="s">
+        <v>68</v>
+      </c>
+      <c r="G6" t="s">
+        <v>72</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>2</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>4000</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6" t="s">
+        <v>70</v>
+      </c>
+      <c r="N6" s="9">
+        <v>42645</v>
+      </c>
+      <c r="O6" t="s">
+        <v>73</v>
+      </c>
+      <c r="P6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B7">
+        <v>5002</v>
+      </c>
+      <c r="C7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" t="s">
+        <v>66</v>
+      </c>
+      <c r="E7" t="s">
+        <v>67</v>
+      </c>
+      <c r="F7" t="s">
+        <v>68</v>
+      </c>
+      <c r="G7" t="s">
+        <v>72</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>3</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>3223</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>100</v>
+      </c>
+      <c r="N7" s="9">
+        <v>42645</v>
+      </c>
+      <c r="O7" t="s">
+        <v>73</v>
+      </c>
+      <c r="P7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B8">
+        <v>5002</v>
+      </c>
+      <c r="C8" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" t="s">
+        <v>66</v>
+      </c>
+      <c r="E8" t="s">
+        <v>67</v>
+      </c>
+      <c r="F8" t="s">
+        <v>68</v>
+      </c>
+      <c r="G8" t="s">
+        <v>74</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>4</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>2142</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8" t="s">
+        <v>70</v>
+      </c>
+      <c r="N8" s="9">
+        <v>42645</v>
+      </c>
+      <c r="O8" t="s">
+        <v>75</v>
+      </c>
+      <c r="P8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B9">
+        <v>5002</v>
+      </c>
+      <c r="C9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" t="s">
+        <v>66</v>
+      </c>
+      <c r="E9" t="s">
+        <v>67</v>
+      </c>
+      <c r="F9" t="s">
+        <v>68</v>
+      </c>
+      <c r="G9" t="s">
+        <v>74</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>5</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>2185</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <v>100</v>
+      </c>
+      <c r="N9" s="9">
+        <v>42645</v>
+      </c>
+      <c r="O9" t="s">
+        <v>75</v>
+      </c>
+      <c r="P9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B10">
+        <v>5002</v>
+      </c>
+      <c r="C10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10" t="s">
+        <v>67</v>
+      </c>
+      <c r="F10" t="s">
+        <v>68</v>
+      </c>
+      <c r="G10" t="s">
+        <v>76</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>6</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <v>2715</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10" t="s">
+        <v>70</v>
+      </c>
+      <c r="N10" s="9">
+        <v>42645</v>
+      </c>
+      <c r="O10" t="s">
+        <v>77</v>
+      </c>
+      <c r="P10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>